<commit_message>
added one more field
Signed-off-by: aakarg <aakar.gupte@eclinicalworks.com>
</commit_message>
<xml_diff>
--- a/Employee_Details.xlsx
+++ b/Employee_Details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -23,40 +23,61 @@
     <t>LASTNAME</t>
   </si>
   <si>
+    <t>E-mail</t>
+  </si>
+  <si>
     <t>kabir</t>
   </si>
   <si>
     <t>khan</t>
   </si>
   <si>
+    <t>kabir.khan@gmail.com</t>
+  </si>
+  <si>
     <t>geetesh</t>
   </si>
   <si>
     <t>chauhan</t>
   </si>
   <si>
+    <t>geet.chauhan@gmail.com</t>
+  </si>
+  <si>
     <t>Sachin</t>
   </si>
   <si>
     <t>Mahajan</t>
   </si>
   <si>
+    <t>sachin.hacker@gmail.com</t>
+  </si>
+  <si>
     <t>Anil</t>
   </si>
   <si>
     <t>Goplani</t>
   </si>
   <si>
+    <t>anil.gops@gmail.com</t>
+  </si>
+  <si>
     <t>Bhavesh</t>
   </si>
   <si>
     <t>parmar</t>
   </si>
   <si>
+    <t>bhav.par@gmail.com</t>
+  </si>
+  <si>
     <t>Mahesh</t>
   </si>
   <si>
     <t>Malsatthar</t>
+  </si>
+  <si>
+    <t>Mahesh.no17@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -117,16 +138,22 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -134,10 +161,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -145,10 +175,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -156,10 +189,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -167,10 +203,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7">
@@ -178,10 +217,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>